<commit_message>
Atualização automática de CAMPO_NOVO.xlsx
</commit_message>
<xml_diff>
--- a/CAMPO_NOVO.xlsx
+++ b/CAMPO_NOVO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9AE926BE-8B4D-4739-AFD3-8BDC6A528B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{12A04C60-91C5-4278-981A-8938BEA5E8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,20 +21,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="5" r:id="rId6"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1065,7 +1052,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1125,36 +1112,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1193,14 +1156,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1246,7 +1204,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{B721BFC1-83D9-4EE5-A942-87D8B1A27756}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{F8815072-EE4D-4033-9857-AE42194FC7EF}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1276,10 +1234,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D118BB63-1332-48F1-9E72-EBC10E7A2C01}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EFE731C-C284-4B7B-8C2C-8719EDD9FC06}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1317,7 +1275,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07A67711-E78E-47C5-893D-40B263155521}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48DF9863-B189-4ABF-A98D-920731B8B8CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1380,7 +1338,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{594B5502-06E6-4A30-8568-BE414AFD99F1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45298A8D-7E1A-441D-B7CF-307AABAEB105}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1399,7 +1357,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88A4BE35-7DC6-868A-0F42-09E51FE49937}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14E51190-7215-D29B-DD08-969291E6347F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1448,7 +1406,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8A2C595-97D1-2839-AA45-8779659D845F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54319DC2-17E3-526D-AC67-6B7DA89E5053}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1467,7 +1425,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2927BAD6-F861-912F-7231-72644C9F403C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE4BC9E9-914D-8FBD-707F-DD3AA3EEA42A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1498,7 +1456,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A266446-BED8-534B-8C45-F9E860280FFF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D4C4E35-43DB-AF4C-CB68-517FEEC31B97}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1529,7 +1487,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D917ED78-AD31-3AF3-2F2E-83B747FDD0C0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F28B563-6F11-3E9C-C808-8C6222FE3D51}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1572,7 +1530,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DE87A64-62ED-4A99-8E2F-27F0409794EE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BAE4E2F-9BB6-4867-A08C-277019D465F1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1610,7 +1568,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B6D6447-5845-496F-AC09-D2E1422ECAD5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA6C0FEC-747D-49C5-8349-8D835059707F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1653,7 +1611,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E773524-A0FC-4FAB-9DD0-F06FE41A09F4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F9981D1-DF61-4E17-8AAF-8FE0CB6A8F56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1966,7 +1924,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C64CAA49-9A47-41EB-80F8-57CC555621BE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239BFDB8-2A2D-4D05-98DC-BD9BC9020F14}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1978,98 +1936,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="37"/>
-    <col min="6" max="6" width="2" style="37" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="37" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="37"/>
+    <col min="1" max="5" width="12.5703125" style="34"/>
+    <col min="6" max="6" width="2" style="34" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="34" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="36"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="36"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="36"/>
+      <c r="F3" s="33"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="36"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="36"/>
+      <c r="F5" s="33"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="36"/>
+      <c r="F6" s="33"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="36"/>
+      <c r="F7" s="33"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="36"/>
+      <c r="F8" s="33"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="36"/>
+      <c r="F9" s="33"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="36"/>
+      <c r="F10" s="33"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="36"/>
+      <c r="F11" s="33"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="36"/>
+      <c r="F12" s="33"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="36"/>
+      <c r="F13" s="33"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="36"/>
+      <c r="F14" s="33"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="36"/>
+      <c r="F15" s="33"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="36"/>
+      <c r="F16" s="33"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="36"/>
+      <c r="F17" s="33"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="36"/>
+      <c r="F18" s="33"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="36"/>
+      <c r="F19" s="33"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="36"/>
+      <c r="F20" s="33"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="36"/>
+      <c r="F21" s="33"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="36"/>
+      <c r="F22" s="33"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="36"/>
+      <c r="F23" s="33"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="36"/>
+      <c r="F24" s="33"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="36"/>
+      <c r="F25" s="33"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="36"/>
+      <c r="F26" s="33"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="36"/>
+      <c r="F27" s="33"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="36"/>
+      <c r="F28" s="33"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="36"/>
+      <c r="F29" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5305,19 +5263,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>270</v>
       </c>
     </row>
@@ -5340,57 +5298,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="19" t="s">
         <v>278</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="19" t="s">
         <v>276</v>
       </c>
     </row>
@@ -5415,54 +5373,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>279</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>280</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>281</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="21" t="s">
         <v>283</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="22" t="s">
         <v>284</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="22" t="s">
         <v>285</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="20" t="s">
         <v>286</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="20" t="s">
         <v>287</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="20" t="s">
         <v>288</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="20" t="s">
         <v>290</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="20" t="s">
         <v>291</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="20" t="s">
         <v>292</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="20" t="s">
         <v>293</v>
       </c>
     </row>
@@ -5473,43 +5432,43 @@
       <c r="B2" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="23">
         <v>45078</v>
       </c>
-      <c r="D2" s="27">
+      <c r="D2" s="24">
         <v>2098</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="24" t="s">
         <v>295</v>
       </c>
-      <c r="F2" s="28">
+      <c r="F2" s="25">
         <v>5228</v>
       </c>
-      <c r="G2" s="28">
+      <c r="G2" s="25">
         <v>628</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="I2" s="26" t="s">
         <v>297</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="26" t="s">
         <v>297</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="26" t="s">
         <v>297</v>
       </c>
-      <c r="M2" s="30" t="s">
+      <c r="M2" s="27" t="s">
         <v>298</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="O2" s="30" t="s">
+      <c r="O2" s="27" t="s">
         <v>298</v>
       </c>
     </row>
@@ -5540,25 +5499,24 @@
       <c r="B1" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="28" t="s">
         <v>300</v>
       </c>
-      <c r="E1" s="32">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="29">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>301</v>
+      </c>
+      <c r="B2" s="32">
         <v>66</v>
       </c>
-      <c r="F1" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
-        <v>301</v>
-      </c>
-      <c r="B2" s="35">
-        <v>66</v>
-      </c>
-      <c r="C2" s="33">
+      <c r="C2" s="30">
         <v>4.3645020499933872E-3</v>
       </c>
     </row>

</xml_diff>